<commit_message>
refactor: change separators for import and export
</commit_message>
<xml_diff>
--- a/public/templates/concept_import.xlsx
+++ b/public/templates/concept_import.xlsx
@@ -61,7 +61,7 @@
     <t>danos</t>
   </si>
   <si>
-    <t>abrasión|Espanhol;abrasion|Inglês;εκτριβή|Grego</t>
+    <t>abrasión~~Espanhol|abrasion~~Inglês|εκτριβή~~Grego</t>
   </si>
   <si>
     <t>amarelecimento</t>
@@ -79,7 +79,7 @@
     <t>Pergaminho</t>
   </si>
   <si>
-    <t>amarillamiento|Espanhol;yellowing|Inglês;κιτρίνισμα|Grego</t>
+    <t>amarillamiento~~Espanhol|yellowing~~Inglês|κιτρίνισμα~~Grego</t>
   </si>
   <si>
     <t>Danos</t>
@@ -100,7 +100,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -475,7 +475,7 @@
     <col min="10" max="10" style="7" width="11.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -507,7 +507,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -537,7 +537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -569,7 +569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>